<commit_message>
02/28 and 03/02 work
</commit_message>
<xml_diff>
--- a/工作日誌.xlsx
+++ b/工作日誌.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a9876\Documents\GitHub\Project_2021_spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DB2132-C067-45B6-A885-0CF443309F7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165ACC12-E9B1-480A-956C-FB3E15615391}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>葉季儒</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>1.優化add title系統</t>
+  </si>
+  <si>
+    <t>1.修復組隊bug(組隊完成顯示未組隊)</t>
+  </si>
+  <si>
+    <t>2.修復後端title傳送錯誤bug</t>
+  </si>
+  <si>
+    <t>3.修復重複註冊問題</t>
+  </si>
+  <si>
+    <t>1.設計註冊介面</t>
   </si>
 </sst>
 </file>
@@ -539,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,6 +911,32 @@
         <v>47</v>
       </c>
     </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
+        <v>44255</v>
+      </c>
+      <c r="D53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>44257</v>
+      </c>
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I1:L1"/>

</xml_diff>

<commit_message>
03/24 work login-page change
</commit_message>
<xml_diff>
--- a/工作日誌.xlsx
+++ b/工作日誌.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Project_2021_Feb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a9876\Documents\GitHub\Project_2021_spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A57EA2-2B92-4380-B87D-6AEC2F5FE7DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3A3A91-720B-4FF6-8A81-9BF854FF8A96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="135">
   <si>
     <t>葉季儒</t>
   </si>
@@ -457,30 +457,39 @@
   <si>
     <t>3.突發事件第二輪設定</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.登入頁面修改</t>
+  </si>
+  <si>
+    <t>2.確保團隊分數正確</t>
+  </si>
+  <si>
+    <t>3.小P 伺服器</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -828,18 +837,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R148"/>
+  <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="M141" sqref="M141"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18">
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,7 +873,7 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18">
       <c r="A3" s="3">
         <v>44236</v>
       </c>
@@ -881,7 +890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -892,22 +901,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18">
       <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18">
       <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18">
       <c r="D7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18">
       <c r="A9" s="3">
         <v>44237</v>
       </c>
@@ -921,12 +930,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18">
       <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18">
       <c r="A12" s="3">
         <v>44242</v>
       </c>
@@ -940,12 +949,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18">
       <c r="E13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18">
       <c r="A15" s="3">
         <v>44243</v>
       </c>
@@ -959,7 +968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18">
       <c r="D16" t="s">
         <v>20</v>
       </c>
@@ -967,7 +976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="3">
         <v>44244</v>
       </c>
@@ -981,12 +990,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="I19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="3">
         <v>44245</v>
       </c>
@@ -1000,12 +1009,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="I22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="3">
         <v>44248</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="D25" t="s">
         <v>25</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="D26" t="s">
         <v>27</v>
       </c>
@@ -1038,12 +1047,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="D27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="3">
         <v>44249</v>
       </c>
@@ -1057,22 +1066,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="I30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="I31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="I32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16">
       <c r="A34" s="3">
         <v>44250</v>
       </c>
@@ -1089,17 +1098,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16">
       <c r="I35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16">
       <c r="I36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16">
       <c r="A38" s="3">
         <v>44251</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16">
       <c r="D39" t="s">
         <v>39</v>
       </c>
@@ -1127,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16">
       <c r="A41" s="3">
         <v>44252</v>
       </c>
@@ -1141,22 +1150,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16">
       <c r="I42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16">
       <c r="I43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16">
       <c r="I44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16">
       <c r="A46" s="3">
         <v>44253</v>
       </c>
@@ -1170,12 +1179,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16">
       <c r="I47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13">
       <c r="A49" s="3">
         <v>44254</v>
       </c>
@@ -1192,12 +1201,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13">
       <c r="I50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13">
       <c r="A53" s="3">
         <v>44255</v>
       </c>
@@ -1208,17 +1217,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13">
       <c r="D54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13">
       <c r="D55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13">
       <c r="A57" s="3">
         <v>44257</v>
       </c>
@@ -1229,7 +1238,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13">
       <c r="A59" s="3">
         <v>44258</v>
       </c>
@@ -1240,12 +1249,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13">
       <c r="D60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13">
       <c r="A62" s="3">
         <v>44264</v>
       </c>
@@ -1262,7 +1271,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13">
       <c r="D63" t="s">
         <v>57</v>
       </c>
@@ -1270,17 +1279,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13">
       <c r="D64" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9">
       <c r="D65" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9">
       <c r="A67" s="3">
         <v>44265</v>
       </c>
@@ -1294,12 +1303,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9">
       <c r="D68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9">
       <c r="A70" s="3">
         <v>44266</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9">
       <c r="D71" t="s">
         <v>64</v>
       </c>
@@ -1321,17 +1330,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9">
       <c r="D72" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9">
       <c r="D73" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9">
       <c r="A75" s="3">
         <v>44267</v>
       </c>
@@ -1345,22 +1354,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9">
       <c r="I76" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9">
       <c r="I77" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9">
       <c r="I78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9">
       <c r="A80" s="3">
         <v>44267</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16">
       <c r="D81" t="s">
         <v>75</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16">
       <c r="A83" s="3">
         <v>44268</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16">
       <c r="D84" t="s">
         <v>87</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16">
       <c r="D85" t="s">
         <v>88</v>
       </c>
@@ -1412,12 +1421,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16">
       <c r="I86" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16">
       <c r="A88" s="3">
         <v>44268</v>
       </c>
@@ -1434,7 +1443,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16">
       <c r="D89" t="s">
         <v>78</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16">
       <c r="D90" t="s">
         <v>85</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16">
       <c r="A92" s="3">
         <v>44269</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16">
       <c r="D93" t="s">
         <v>94</v>
       </c>
@@ -1478,22 +1487,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16">
       <c r="I94" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16">
       <c r="I95" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16">
       <c r="I96" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16">
       <c r="A98" s="3">
         <v>44269</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16">
       <c r="D99" t="s">
         <v>92</v>
       </c>
@@ -1521,7 +1530,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16">
       <c r="I100" t="s">
         <v>83</v>
       </c>
@@ -1529,12 +1538,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16">
       <c r="P101" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16">
       <c r="A103" s="3">
         <v>44270</v>
       </c>
@@ -1548,27 +1557,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16">
       <c r="I104" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16">
       <c r="I105" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16">
       <c r="I106" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16">
       <c r="I107" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16">
       <c r="A109" s="3">
         <v>44271</v>
       </c>
@@ -1582,17 +1591,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16">
       <c r="I110" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16">
       <c r="I111" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16">
       <c r="A113" s="3">
         <v>44271</v>
       </c>
@@ -1609,7 +1618,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16">
       <c r="I114" t="s">
         <v>102</v>
       </c>
@@ -1617,22 +1626,22 @@
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16">
       <c r="I115" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16">
       <c r="I116" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16">
       <c r="I117" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16">
       <c r="A119" s="3">
         <v>44272</v>
       </c>
@@ -1646,12 +1655,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16">
       <c r="I120" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16">
       <c r="A122" s="3">
         <v>44274</v>
       </c>
@@ -1665,22 +1674,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16">
       <c r="I123" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16">
       <c r="I124" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16">
       <c r="I125" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16">
       <c r="A127" s="3">
         <v>44274</v>
       </c>
@@ -1697,7 +1706,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16">
       <c r="I128" t="s">
         <v>114</v>
       </c>
@@ -1705,7 +1714,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16">
       <c r="I129" t="s">
         <v>115</v>
       </c>
@@ -1713,17 +1722,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16">
       <c r="I130" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16">
       <c r="I131" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16">
       <c r="A133" s="3">
         <v>44275</v>
       </c>
@@ -1737,22 +1746,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16">
       <c r="I134" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16">
       <c r="I135" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16">
       <c r="I136" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16">
       <c r="A138" s="3">
         <v>44276</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16">
       <c r="D139" t="s">
         <v>123</v>
       </c>
@@ -1780,7 +1789,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16">
       <c r="D140" t="s">
         <v>124</v>
       </c>
@@ -1788,17 +1797,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16">
       <c r="P141" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16">
       <c r="P142" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16">
       <c r="A144" s="3">
         <v>44277</v>
       </c>
@@ -1815,7 +1824,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="9:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16">
       <c r="I145" t="s">
         <v>126</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="146" spans="9:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16">
       <c r="I146" t="s">
         <v>131</v>
       </c>
@@ -1831,14 +1840,38 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="9:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16">
       <c r="P147" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="148" spans="9:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16">
       <c r="P148" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16">
+      <c r="A150" s="3">
+        <v>44277</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="D150" t="s">
+        <v>132</v>
+      </c>
+      <c r="I150" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16">
+      <c r="I151" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
+      <c r="I152" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>